<commit_message>
Import Order Function Changed
</commit_message>
<xml_diff>
--- a/dtd_asset/order_sample.xlsx
+++ b/dtd_asset/order_sample.xlsx
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
-  <si>
-    <t>customer_email</t>
-  </si>
-  <si>
-    <t>vendor_email</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>reciepent</t>
   </si>
@@ -59,45 +53,35 @@
     <t>memo</t>
   </si>
   <si>
-    <t>Chirag Bhatt</t>
-  </si>
-  <si>
-    <t>Naval Nagar</t>
-  </si>
-  <si>
     <t>Medium Box</t>
   </si>
   <si>
     <t>Testing</t>
   </si>
   <si>
-    <t>vimalghorecha@gmail.com</t>
-  </si>
-  <si>
-    <t>chiragbhattmca@gmail.com</t>
-  </si>
-  <si>
-    <t>vimalghorecha@gmail.com11</t>
-  </si>
-  <si>
-    <t>chiragbhattmca@gmail.com11</t>
+    <t>Mehul Shukla</t>
+  </si>
+  <si>
+    <t>Swaminaray Chowk</t>
+  </si>
+  <si>
+    <t>Hardik Maheta</t>
+  </si>
+  <si>
+    <t>Wankaner</t>
+  </si>
+  <si>
+    <t>Short Box</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
@@ -119,16 +103,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -407,7 +388,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -415,19 +396,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,84 +435,60 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>360004</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>9033404578</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="G2" t="s">
         <v>10</v>
       </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>360004</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>9033404578</v>
+      </c>
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2">
-        <v>360004</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>9033404578</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>360004</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>9033404578</v>
+      <c r="G3" t="s">
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="B3" r:id="rId4"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>